<commit_message>
Likert Scale Implementation for COMP-101
</commit_message>
<xml_diff>
--- a/src/ACAT/grades/grades_101.xlsx
+++ b/src/ACAT/grades/grades_101.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Raghava_Master's\Professional Seminar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A48942E0-407B-4906-8405-60D3C6DAD0B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FC27239-D9C9-449F-8A89-B54DC68A499A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{2C41E5BC-1DA1-48A2-BE0D-00875B461B44}"/>
   </bookViews>
@@ -36,9 +36,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
-    <t xml:space="preserve">Student ID     </t>
-  </si>
-  <si>
     <t>Final Exam</t>
   </si>
   <si>
@@ -55,6 +52,9 @@
   </si>
   <si>
     <t xml:space="preserve"> Final Project</t>
+  </si>
+  <si>
+    <t>SIS User ID</t>
   </si>
 </sst>
 </file>
@@ -440,9 +440,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49CCB1BA-52E2-4870-927B-7E4F574FFA77}">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
@@ -457,25 +455,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7">

</xml_diff>